<commit_message>
Added a dog body background when showing organs Added a cardio respiratory system
</commit_message>
<xml_diff>
--- a/StreamingAssets/BodyParts.xlsx
+++ b/StreamingAssets/BodyParts.xlsx
@@ -413,6 +413,9 @@
     <t>Trachea</t>
   </si>
   <si>
+    <t>Diaphragme</t>
+  </si>
+  <si>
     <t>Digestive_system pancreas</t>
   </si>
   <si>
@@ -471,9 +474,6 @@
   </si>
   <si>
     <t>VessieM</t>
-  </si>
-  <si>
-    <t>Diaphragme</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1199,162 +1199,182 @@
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>135</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>137</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>138</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>132</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>